<commit_message>
Added UART/USB, JTAG, I2C outputs for programming
</commit_message>
<xml_diff>
--- a/BrushedMotorBoard/BOM/BoM.xlsx
+++ b/BrushedMotorBoard/BOM/BoM.xlsx
@@ -400,7 +400,7 @@
         </is>
       </c>
       <c t="n" r="K3">
-        <v>233813</v>
+        <v>233027</v>
       </c>
       <c t="inlineStr" r="L3">
         <is>
@@ -476,7 +476,7 @@
         </is>
       </c>
       <c t="n" r="K4">
-        <v>704455</v>
+        <v>701455</v>
       </c>
       <c t="inlineStr" r="L4">
         <is>
@@ -769,14 +769,14 @@
         </is>
       </c>
       <c t="n" r="H8">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c t="n" r="I8">
         <v>0.42000</v>
       </c>
       <c t="inlineStr" r="J8">
         <is>
-          <t>$2.52</t>
+          <t>$1.68</t>
         </is>
       </c>
       <c t="n" r="K8">
@@ -921,14 +921,14 @@
         </is>
       </c>
       <c t="n" r="H10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c t="n" r="I10">
         <v>0.92000</v>
       </c>
       <c t="inlineStr" r="J10">
         <is>
-          <t>$1.84</t>
+          <t>$0.92</t>
         </is>
       </c>
       <c t="n" r="K10">
@@ -1033,6 +1033,82 @@
       <c t="inlineStr" r="P11">
         <is>
           <t>Not Available</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c t="inlineStr" r="A12">
+        <is>
+          <t>0022232041</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="B12">
+        <is>
+          <t>Molex, LLC</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C12">
+        <is>
+          <t>WM4202-ND</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="D12">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c t="inlineStr" r="E12">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c t="inlineStr" r="F12">
+        <is>
+          <t>Bulk</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G12">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c t="n" r="H12">
+        <v>2</v>
+      </c>
+      <c t="n" r="I12">
+        <v>0.28000</v>
+      </c>
+      <c t="inlineStr" r="J12">
+        <is>
+          <t>$0.56</t>
+        </is>
+      </c>
+      <c t="n" r="K12">
+        <v>51523</v>
+      </c>
+      <c t="inlineStr" r="L12">
+        <is>
+          <t>7 Weeks</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="M12">
+        <is>
+          <t>CONN HEADER 4POS .100 VERT TIN</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="N12">
+        <is>
+          <t>RoHS Compliant</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="O12">
+        <is>
+          <t>Lead free</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="P12">
+        <is>
+          <t>REACH Unaffected</t>
         </is>
       </c>
     </row>

</xml_diff>